<commit_message>
Author : Ruchit Jain Description : Updated Task breakdown sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RuchitJain.xlsx
+++ b/TeamDetails/TasksBreakDown/RuchitJain.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
   <si>
     <t>Story ID</t>
   </si>
@@ -52,9 +52,6 @@
     <t>T01</t>
   </si>
   <si>
-    <t xml:space="preserve">Designing select menu and upload button </t>
-  </si>
-  <si>
     <t>T02</t>
   </si>
   <si>
@@ -64,18 +61,9 @@
     <t>T03</t>
   </si>
   <si>
-    <t xml:space="preserve">Designing controller of Angular </t>
-  </si>
-  <si>
     <t>SSDMS 46</t>
   </si>
   <si>
-    <t xml:space="preserve">Saving selected csv on local machine </t>
-  </si>
-  <si>
-    <t>Checking type of CSV(comparing column names)</t>
-  </si>
-  <si>
     <t>T04</t>
   </si>
   <si>
@@ -127,9 +115,6 @@
     <t>T13</t>
   </si>
   <si>
-    <t xml:space="preserve">Integrating all modules with proper flow </t>
-  </si>
-  <si>
     <t>T14</t>
   </si>
   <si>
@@ -139,42 +124,12 @@
     <t>T15</t>
   </si>
   <si>
-    <t>Debugging</t>
-  </si>
-  <si>
     <t>Create controller</t>
   </si>
   <si>
-    <t>Validating Candidate.csv</t>
-  </si>
-  <si>
-    <t>Validating Batch.csv</t>
-  </si>
-  <si>
-    <t>Validating Training_Partner.csv</t>
-  </si>
-  <si>
-    <t>Validating Centre.csv</t>
-  </si>
-  <si>
-    <t>Validating Trainer.csv</t>
-  </si>
-  <si>
-    <t>Validating Assessment_Agency.csv</t>
-  </si>
-  <si>
-    <t>Validating Assessor.csv</t>
-  </si>
-  <si>
-    <t>Validating Employer.csv</t>
-  </si>
-  <si>
     <t>T16</t>
   </si>
   <si>
-    <t>Coding DAO for each CSV</t>
-  </si>
-  <si>
     <t>T17</t>
   </si>
   <si>
@@ -190,37 +145,100 @@
     <t>T21</t>
   </si>
   <si>
-    <t>Coding DAO for all 4 tables to fetch data</t>
-  </si>
-  <si>
-    <t>Integrating data of all 4 tables in single object in service</t>
-  </si>
-  <si>
     <t>Create controller &amp; Service</t>
   </si>
   <si>
     <t xml:space="preserve">Program functionality of accept/reject/show interest button </t>
   </si>
   <si>
-    <t>Coding respective DAO's for accept/reject/show interest functionality</t>
-  </si>
-  <si>
     <t>Program to fetch data from different tables + Creating SQL queries</t>
   </si>
   <si>
-    <t>Integrating all modules with proper flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding config class and .yml file </t>
-  </si>
-  <si>
     <t>Unit Testing</t>
   </si>
   <si>
-    <t>Understanding exact Work flow of story</t>
-  </si>
-  <si>
     <t>SSDMS16, SSDMS17, SSDMS18, SSDMS19, SSDMS20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design select menu and upload button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design controller of Angular </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save selected csv on local machine </t>
+  </si>
+  <si>
+    <t>Check type of CSV(comparing column names)</t>
+  </si>
+  <si>
+    <t>Validate Candidate.csv</t>
+  </si>
+  <si>
+    <t>Validate Batch.csv</t>
+  </si>
+  <si>
+    <t>Validate Training_Partner.csv</t>
+  </si>
+  <si>
+    <t>Validate Centre.csv</t>
+  </si>
+  <si>
+    <t>Validate Trainer.csv</t>
+  </si>
+  <si>
+    <t>Validate Assessment_Agency.csv</t>
+  </si>
+  <si>
+    <t>Validate Assessor.csv</t>
+  </si>
+  <si>
+    <t>Validate Employer.csv</t>
+  </si>
+  <si>
+    <t>Code DAO for each CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrate all modules with proper flow </t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand &amp; Design UI grid for tables </t>
+  </si>
+  <si>
+    <t>TO2</t>
+  </si>
+  <si>
+    <t>Fit the designed table in their suitable frames</t>
+  </si>
+  <si>
+    <t>TO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create controller of angular </t>
+  </si>
+  <si>
+    <t>Understand exact Work flow of story</t>
+  </si>
+  <si>
+    <t>Code DAO for all 4 tables to fetch data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code config class and .yml file </t>
+  </si>
+  <si>
+    <t>Integrate data of all 4 tables in single object in service</t>
+  </si>
+  <si>
+    <t>Code respective DAO's for accept/reject/show interest functionality</t>
+  </si>
+  <si>
+    <t>Integrate all modules with proper flow</t>
+  </si>
+  <si>
+    <t>Buffer</t>
   </si>
 </sst>
 </file>
@@ -258,7 +276,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -282,47 +300,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -337,15 +327,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2927,15 +2916,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G46"/>
+  <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" customWidth="1"/>
     <col min="4" max="4" width="67.44140625" style="1" customWidth="1"/>
@@ -2975,770 +2964,826 @@
         <f>SUM(E3:E5)</f>
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <f>E3-F3</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G28" si="0">E4-F4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G46" si="0">E4-F4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <f>SUM(E7:E28)</f>
         <v>41</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="2">
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="6">
+        <f>SUM(E32:E46)</f>
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36">
         <v>1</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f>E36-F36</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2">
+    <row r="37" spans="1:7">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37">
         <v>2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <f>E37-F37</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38">
         <v>1</v>
       </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2">
-        <v>3</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="2">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <f>E21-F21</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <f>E22-F22</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <f>E23-F23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="2">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <f>E24-F24</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="2">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0</v>
-      </c>
-      <c r="G25" s="2">
-        <f>E25-F25</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <f>E26-F26</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="2">
-        <v>2</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0</v>
-      </c>
-      <c r="G27" s="2">
-        <f>E27-F27</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2">
-        <f>E28-F28</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="7">
-        <f>SUM(E32:E42)</f>
-        <v>22</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="2">
-        <v>2</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="2">
-        <v>3</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2">
-        <f>E35-F35</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" s="2">
-        <v>3</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <f>E36-F36</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="2">
-        <v>3</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <f>E37-F37</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2">
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
         <f>E38-F38</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ref="G39:G46" si="1">E39-F39</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E46">
         <v>2</v>
       </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <f>E39-F39</f>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="2">
-        <v>2</v>
-      </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2">
-        <f>E40-F40</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="2">
-        <v>2</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2">
-        <f>E41-F41</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="2">
-        <v>2</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2">
-        <f>E42-F42</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+    <row r="47" spans="1:7">
+      <c r="A47" s="8"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B32:B46"/>
+    <mergeCell ref="A32:A46"/>
     <mergeCell ref="A7:A28"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B7:B28"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B32:B42"/>
-    <mergeCell ref="A32:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author : Ruchit Description : Updated Task Breakdown List
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RuchitJain.xlsx
+++ b/TeamDetails/TasksBreakDown/RuchitJain.xlsx
@@ -328,13 +328,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +608,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2918,8 +2918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2957,10 +2957,10 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <f>SUM(E3:E5)</f>
         <v>7</v>
       </c>
@@ -2982,8 +2982,8 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -3002,8 +3002,8 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -3025,10 +3025,10 @@
       <c r="D6"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="7">
         <f>SUM(E7:E28)</f>
         <v>41</v>
       </c>
@@ -3050,8 +3050,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -3062,16 +3062,16 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -3082,16 +3082,16 @@
         <v>4</v>
       </c>
       <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -3102,16 +3102,16 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -3121,8 +3121,8 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" t="s">
         <v>15</v>
       </c>
@@ -3141,8 +3141,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" t="s">
         <v>16</v>
       </c>
@@ -3161,8 +3161,8 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -3181,8 +3181,8 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -3201,8 +3201,8 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -3221,8 +3221,8 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -3241,8 +3241,8 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
       <c r="C18" t="s">
         <v>26</v>
       </c>
@@ -3261,8 +3261,8 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" t="s">
         <v>27</v>
       </c>
@@ -3281,8 +3281,8 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>29</v>
       </c>
@@ -3301,8 +3301,8 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
       <c r="C21" t="s">
         <v>30</v>
       </c>
@@ -3321,8 +3321,8 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -3341,8 +3341,8 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
       <c r="C23" t="s">
         <v>34</v>
       </c>
@@ -3361,8 +3361,8 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
       <c r="C24" t="s">
         <v>35</v>
       </c>
@@ -3381,8 +3381,8 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
       <c r="C25" t="s">
         <v>36</v>
       </c>
@@ -3401,8 +3401,8 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
       <c r="C26" t="s">
         <v>37</v>
       </c>
@@ -3421,8 +3421,8 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
       <c r="C27" t="s">
         <v>38</v>
       </c>
@@ -3441,8 +3441,8 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
       <c r="C28" t="s">
         <v>39</v>
       </c>
@@ -3470,10 +3470,10 @@
       <c r="D31"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="7">
         <f>SUM(E32:E46)</f>
         <v>29</v>
       </c>
@@ -3494,8 +3494,8 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
       <c r="C33" t="s">
         <v>61</v>
       </c>
@@ -3513,8 +3513,8 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
       <c r="C34" t="s">
         <v>63</v>
       </c>
@@ -3532,8 +3532,8 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
       <c r="C35" t="s">
         <v>13</v>
       </c>
@@ -3551,8 +3551,8 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
       <c r="C36" t="s">
         <v>15</v>
       </c>
@@ -3571,8 +3571,8 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
       <c r="C37" t="s">
         <v>16</v>
       </c>
@@ -3591,8 +3591,8 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
       <c r="C38" t="s">
         <v>18</v>
       </c>
@@ -3611,8 +3611,8 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
       <c r="C39" t="s">
         <v>22</v>
       </c>
@@ -3631,8 +3631,8 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
       <c r="C40" t="s">
         <v>23</v>
       </c>
@@ -3651,8 +3651,8 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
       <c r="C41" t="s">
         <v>24</v>
       </c>
@@ -3671,8 +3671,8 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
       <c r="C42" t="s">
         <v>26</v>
       </c>
@@ -3691,8 +3691,8 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
       <c r="C43" t="s">
         <v>27</v>
       </c>
@@ -3711,8 +3711,8 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
       <c r="C44" t="s">
         <v>29</v>
       </c>
@@ -3731,8 +3731,8 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
       <c r="C45" t="s">
         <v>30</v>
       </c>
@@ -3751,8 +3751,8 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
       <c r="C46" t="s">
         <v>32</v>
       </c>
@@ -3771,10 +3771,10 @@
       </c>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="8"/>
+      <c r="A47" s="6"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="8"/>
+      <c r="A48" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Author : Ruchit Jain Description: Updated Task Breakdown List (Added a buffer time of 2 hours in data import story)
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RuchitJain.xlsx
+++ b/TeamDetails/TasksBreakDown/RuchitJain.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>Story ID</t>
   </si>
@@ -239,13 +239,25 @@
   </si>
   <si>
     <t>Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status </t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>Complete by 6th July 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +273,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,8 +293,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -308,11 +350,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -335,6 +386,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2916,10 +2978,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G48"/>
+  <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2931,9 +2993,10 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2955,8 +3018,11 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
@@ -2981,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" t="s">
@@ -2997,11 +3063,11 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G28" si="0">E4-F4</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <f t="shared" ref="G4:G29" si="0">E4-F4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" t="s">
@@ -3016,15 +3082,19 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="D6"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="13">
+        <f>SUM(G3:G5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -3042,14 +3112,17 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" t="s">
@@ -3068,8 +3141,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" t="s">
@@ -3082,14 +3156,15 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" t="s">
@@ -3108,8 +3183,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="D11" t="s">
@@ -3119,8 +3195,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" t="s">
@@ -3139,8 +3216,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" t="s">
@@ -3159,8 +3237,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" t="s">
@@ -3179,8 +3258,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" t="s">
@@ -3199,8 +3279,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" t="s">
@@ -3219,8 +3300,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" t="s">
@@ -3239,8 +3321,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" t="s">
@@ -3259,8 +3342,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" t="s">
@@ -3279,8 +3363,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" t="s">
@@ -3299,8 +3384,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" t="s">
@@ -3313,14 +3399,15 @@
         <v>0.5</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" t="s">
@@ -3339,8 +3426,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" t="s">
@@ -3359,8 +3447,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" t="s">
@@ -3379,8 +3468,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" t="s">
@@ -3393,14 +3485,15 @@
         <v>3</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>2</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" t="s">
@@ -3419,8 +3512,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" t="s">
@@ -3439,8 +3533,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" t="s">
@@ -3455,21 +3550,42 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="D29"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="G28" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="D30"/>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="G30" s="12">
+        <f>SUM(G7:G29)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:8">
       <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
@@ -3772,12 +3888,18 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="6"/>
+      <c r="G47" s="13">
+        <f>SUM(G32:G46)</f>
+        <v>29</v>
+      </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="H7:H23"/>
+    <mergeCell ref="H24:H29"/>
     <mergeCell ref="B32:B46"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A7:A28"/>

</xml_diff>

<commit_message>
Author : Ruchit Description : Task Breakdown updated sheet. (Extended buffer time from 2 hours to 6 hours in story ID SSDMS 46)
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RuchitJain.xlsx
+++ b/TeamDetails/TasksBreakDown/RuchitJain.xlsx
@@ -250,7 +250,7 @@
     <t>T22</t>
   </si>
   <si>
-    <t>Complete by 6th July 2017</t>
+    <t>Complete by 7th July 2017</t>
   </si>
 </sst>
 </file>
@@ -381,22 +381,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2980,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3023,10 +3023,10 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="15">
         <f>SUM(E3:E5)</f>
         <v>7</v>
       </c>
@@ -3048,8 +3048,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -3068,8 +3068,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -3082,23 +3082,23 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="11">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="D6"/>
-      <c r="G6" s="13">
+      <c r="G6" s="10">
         <f>SUM(G3:G5)</f>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="14">
         <f>SUM(E7:E28)</f>
         <v>41</v>
       </c>
@@ -3118,13 +3118,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -3141,11 +3141,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -3162,11 +3162,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -3183,11 +3183,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -3195,11 +3195,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" t="s">
         <v>15</v>
       </c>
@@ -3216,11 +3216,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
       <c r="C13" t="s">
         <v>16</v>
       </c>
@@ -3237,11 +3237,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="9"/>
+      <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -3258,11 +3258,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -3279,11 +3279,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -3300,11 +3300,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="9"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -3321,11 +3321,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="9"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
       <c r="C18" t="s">
         <v>26</v>
       </c>
@@ -3342,11 +3342,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="9"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
       <c r="C19" t="s">
         <v>27</v>
       </c>
@@ -3363,11 +3363,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="9"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
       <c r="C20" t="s">
         <v>29</v>
       </c>
@@ -3384,11 +3384,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
       <c r="C21" t="s">
         <v>30</v>
       </c>
@@ -3405,11 +3405,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="9"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -3426,11 +3426,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="9"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
       <c r="C23" t="s">
         <v>34</v>
       </c>
@@ -3447,11 +3447,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="9"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
       <c r="C24" t="s">
         <v>35</v>
       </c>
@@ -3462,19 +3462,19 @@
         <v>5</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H24" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
       <c r="C25" t="s">
         <v>36</v>
       </c>
@@ -3485,17 +3485,17 @@
         <v>3</v>
       </c>
       <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G25">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
       <c r="C26" t="s">
         <v>37</v>
       </c>
@@ -3512,11 +3512,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H26" s="15"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
       <c r="C27" t="s">
         <v>38</v>
       </c>
@@ -3533,11 +3533,11 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
       <c r="C28" t="s">
         <v>39</v>
       </c>
@@ -3550,11 +3550,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="7">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H28" s="15"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
       <c r="C29" t="s">
@@ -3564,32 +3564,32 @@
         <v>71</v>
       </c>
       <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29">
         <v>2</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29" s="11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H29" s="15"/>
+      <c r="G29" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
       <c r="D30"/>
-      <c r="G30" s="12">
+      <c r="G30" s="9">
         <f>SUM(G7:G29)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="D31"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="14">
         <f>SUM(E32:E46)</f>
         <v>29</v>
       </c>
@@ -3610,8 +3610,8 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
       <c r="C33" t="s">
         <v>61</v>
       </c>
@@ -3629,8 +3629,8 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
       <c r="C34" t="s">
         <v>63</v>
       </c>
@@ -3648,8 +3648,8 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
       <c r="C35" t="s">
         <v>13</v>
       </c>
@@ -3667,8 +3667,8 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
       <c r="C36" t="s">
         <v>15</v>
       </c>
@@ -3687,8 +3687,8 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
       <c r="C37" t="s">
         <v>16</v>
       </c>
@@ -3707,8 +3707,8 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
       <c r="C38" t="s">
         <v>18</v>
       </c>
@@ -3727,8 +3727,8 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
       <c r="C39" t="s">
         <v>22</v>
       </c>
@@ -3747,8 +3747,8 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
       <c r="C40" t="s">
         <v>23</v>
       </c>
@@ -3767,8 +3767,8 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
       <c r="C41" t="s">
         <v>24</v>
       </c>
@@ -3787,8 +3787,8 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
       <c r="C42" t="s">
         <v>26</v>
       </c>
@@ -3807,8 +3807,8 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
       <c r="C43" t="s">
         <v>27</v>
       </c>
@@ -3827,8 +3827,8 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
       <c r="C44" t="s">
         <v>29</v>
       </c>
@@ -3847,8 +3847,8 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="14"/>
       <c r="C45" t="s">
         <v>30</v>
       </c>
@@ -3867,8 +3867,8 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
       <c r="C46" t="s">
         <v>32</v>
       </c>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="6"/>
-      <c r="G47" s="13">
+      <c r="G47" s="10">
         <f>SUM(G32:G46)</f>
         <v>29</v>
       </c>
@@ -3898,14 +3898,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B7:B28"/>
+    <mergeCell ref="B3:B5"/>
     <mergeCell ref="H7:H23"/>
     <mergeCell ref="H24:H29"/>
     <mergeCell ref="B32:B46"/>
     <mergeCell ref="A32:A46"/>
     <mergeCell ref="A7:A28"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B7:B28"/>
-    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author : Ruchit Jain Description : Updated Task BreakDown List
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RuchitJain.xlsx
+++ b/TeamDetails/TasksBreakDown/RuchitJain.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
   <si>
     <t>Story ID</t>
   </si>
@@ -248,16 +248,13 @@
   </si>
   <si>
     <t>T22</t>
-  </si>
-  <si>
-    <t>Complete by 7th July 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,14 +270,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,18 +293,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -385,17 +364,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -670,7 +645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2980,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3023,10 +2998,10 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="11">
         <f>SUM(E3:E5)</f>
         <v>7</v>
       </c>
@@ -3048,8 +3023,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -3068,8 +3043,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -3082,7 +3057,7 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3095,10 +3070,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="12">
         <f>SUM(E7:E28)</f>
         <v>41</v>
       </c>
@@ -3118,13 +3093,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -3141,11 +3116,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" t="s">
         <v>11</v>
       </c>
@@ -3162,11 +3137,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="12"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
@@ -3183,11 +3158,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -3195,11 +3170,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" t="s">
         <v>15</v>
       </c>
@@ -3216,11 +3191,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" t="s">
         <v>16</v>
       </c>
@@ -3237,11 +3212,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="12"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" t="s">
         <v>18</v>
       </c>
@@ -3258,11 +3233,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" t="s">
         <v>22</v>
       </c>
@@ -3279,11 +3254,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="12"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" t="s">
         <v>23</v>
       </c>
@@ -3300,11 +3275,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -3321,11 +3296,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" t="s">
         <v>26</v>
       </c>
@@ -3342,11 +3317,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="12"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" t="s">
         <v>27</v>
       </c>
@@ -3363,11 +3338,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" t="s">
         <v>29</v>
       </c>
@@ -3384,11 +3359,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="12"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
       <c r="C21" t="s">
         <v>30</v>
       </c>
@@ -3405,11 +3380,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="12"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -3426,11 +3401,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
       <c r="C23" t="s">
         <v>34</v>
       </c>
@@ -3447,11 +3422,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" t="s">
         <v>35</v>
       </c>
@@ -3468,13 +3443,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>75</v>
-      </c>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
       <c r="C25" t="s">
         <v>36</v>
       </c>
@@ -3488,14 +3461,13 @@
         <v>2</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
       <c r="C26" t="s">
         <v>37</v>
       </c>
@@ -3509,14 +3481,13 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
       <c r="C27" t="s">
         <v>38</v>
       </c>
@@ -3530,14 +3501,13 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" t="s">
         <v>39</v>
       </c>
@@ -3551,8 +3521,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H28" s="13"/>
     </row>
@@ -3570,8 +3539,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H29" s="13"/>
     </row>
@@ -3579,17 +3547,17 @@
       <c r="D30"/>
       <c r="G30" s="9">
         <f>SUM(G7:G29)</f>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="D31"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="12">
         <f>SUM(E32:E46)</f>
         <v>29</v>
       </c>
@@ -3610,8 +3578,8 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" t="s">
         <v>61</v>
       </c>
@@ -3629,8 +3597,8 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" t="s">
         <v>63</v>
       </c>
@@ -3648,8 +3616,8 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
       <c r="C35" t="s">
         <v>13</v>
       </c>
@@ -3667,8 +3635,8 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
       <c r="C36" t="s">
         <v>15</v>
       </c>
@@ -3687,8 +3655,8 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
       <c r="C37" t="s">
         <v>16</v>
       </c>
@@ -3707,8 +3675,8 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" t="s">
         <v>18</v>
       </c>
@@ -3727,8 +3695,8 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" t="s">
         <v>22</v>
       </c>
@@ -3747,8 +3715,8 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
       <c r="C40" t="s">
         <v>23</v>
       </c>
@@ -3767,8 +3735,8 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
       <c r="C41" t="s">
         <v>24</v>
       </c>
@@ -3787,8 +3755,8 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
       <c r="C42" t="s">
         <v>26</v>
       </c>
@@ -3807,8 +3775,8 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
       <c r="C43" t="s">
         <v>27</v>
       </c>
@@ -3827,8 +3795,8 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
       <c r="C44" t="s">
         <v>29</v>
       </c>
@@ -3847,8 +3815,8 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
       <c r="C45" t="s">
         <v>30</v>
       </c>
@@ -3867,8 +3835,8 @@
       </c>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
       <c r="C46" t="s">
         <v>32</v>
       </c>
@@ -3897,15 +3865,14 @@
       <c r="A48" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
+    <mergeCell ref="B32:B46"/>
+    <mergeCell ref="A32:A46"/>
+    <mergeCell ref="A7:A28"/>
+    <mergeCell ref="H7:H29"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B7:B28"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="H7:H23"/>
-    <mergeCell ref="H24:H29"/>
-    <mergeCell ref="B32:B46"/>
-    <mergeCell ref="A32:A46"/>
-    <mergeCell ref="A7:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>